<commit_message>
Fix contracts import excel test
</commit_message>
<xml_diff>
--- a/server/test/data/contracts.xlsx
+++ b/server/test/data/contracts.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
     <workbookView xWindow="630" yWindow="555" windowWidth="27495" windowHeight="14250"/>
@@ -109,9 +109,6 @@
     <t>Petrobras</t>
   </si>
   <si>
-    <t>Gás</t>
-  </si>
-  <si>
     <t>Objeto</t>
   </si>
   <si>
@@ -128,6 +125,9 @@
   </si>
   <si>
     <t>Euro</t>
+  </si>
+  <si>
+    <t>Produção</t>
   </si>
 </sst>
 </file>
@@ -504,8 +504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -559,10 +559,10 @@
         <v>11</v>
       </c>
       <c r="M1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -597,7 +597,7 @@
         <v>18</v>
       </c>
       <c r="N2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -629,7 +629,7 @@
         <v>23</v>
       </c>
       <c r="N3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -661,7 +661,7 @@
         <v>12</v>
       </c>
       <c r="N4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -690,7 +690,7 @@
         <v>30</v>
       </c>
       <c r="I5" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="J5" t="s">
         <v>17</v>
@@ -702,10 +702,10 @@
         <v>1792051158</v>
       </c>
       <c r="M5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding field "type" to Contract
</commit_message>
<xml_diff>
--- a/server/test/data/contracts.xlsx
+++ b/server/test/data/contracts.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Pasta principal" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="42">
   <si>
     <t>Identificador</t>
   </si>
@@ -128,6 +128,18 @@
   </si>
   <si>
     <t>Produção</t>
+  </si>
+  <si>
+    <t>tipo</t>
+  </si>
+  <si>
+    <t>NÃO</t>
+  </si>
+  <si>
+    <t>CAPEX</t>
+  </si>
+  <si>
+    <t>opex</t>
   </si>
 </sst>
 </file>
@@ -502,17 +514,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N5"/>
+  <dimension ref="A1:O5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="37.125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="45" customWidth="1"/>
+    <col min="4" max="4" width="65" customWidth="1"/>
     <col min="5" max="5" width="15.125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="27.75" customWidth="1"/>
@@ -521,7 +533,7 @@
     <col min="13" max="13" width="19.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -564,8 +576,11 @@
       <c r="N1" t="s">
         <v>33</v>
       </c>
+      <c r="O1" t="s">
+        <v>38</v>
+      </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -599,8 +614,11 @@
       <c r="N2" t="s">
         <v>34</v>
       </c>
+      <c r="O2" t="s">
+        <v>39</v>
+      </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -631,8 +649,11 @@
       <c r="N3" t="s">
         <v>34</v>
       </c>
+      <c r="O3" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -663,8 +684,11 @@
       <c r="N4" t="s">
         <v>35</v>
       </c>
+      <c r="O4" t="s">
+        <v>41</v>
+      </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>250</v>
       </c>

</xml_diff>

<commit_message>
Testing contracts excel import
</commit_message>
<xml_diff>
--- a/server/test/data/contracts.xlsx
+++ b/server/test/data/contracts.xlsx
@@ -684,9 +684,6 @@
       <c r="N4" t="s">
         <v>35</v>
       </c>
-      <c r="O4" t="s">
-        <v>41</v>
-      </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -730,6 +727,9 @@
       </c>
       <c r="N5" t="s">
         <v>36</v>
+      </c>
+      <c r="O5" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>